<commit_message>
Updated result in execl
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\research\CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4BF45C-FC8E-4AE0-9102-50D7A9DA99B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB20267-6DC0-459B-B82A-65378D1B14A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,13 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>noBlock_singleThread</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Kernel time (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>noBlock_multiThread (8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>noBlock_multiThread (64)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -357,15 +365,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="21.9140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -379,7 +387,23 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>648.62699999999995</v>
+        <v>2876184.915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1149000.395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1091610.7679999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated loop unrolling result.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\research\CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55531C75-FD96-4FCA-9DC0-AF0F56407AFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC4E3C8-EBF3-4665-BFC8-2DAD21C81B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>noBlock_singleThread</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +56,10 @@
   </si>
   <si>
     <t>Kernel time (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop unrolling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -79,12 +83,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,11 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -384,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -396,140 +407,170 @@
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.9140625" customWidth="1"/>
+    <col min="10" max="10" width="13.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10">
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>2876184.915</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>49175.35</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="J3">
+        <v>2817.8130000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>1149000.395</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>6597.8890000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
+      <c r="J4">
+        <v>461.50299999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>1091610.7679999999</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>8</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>5134.2669999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="E5">
+      <c r="J5">
+        <v>374.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="E6">
         <v>16</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>16</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>16</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>6027.4160000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="E7">
+      <c r="J6">
+        <v>380.839</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="E8">
         <v>8</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>8</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>64</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>6140.1120000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="D8" s="1"/>
-      <c r="E8">
+      <c r="J8">
+        <v>398.89299999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="D9" s="1"/>
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>32</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>5153.28</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="E9">
+      <c r="J9">
+        <v>377.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>2</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>16</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>6513.1080000000002</v>
+      </c>
+      <c r="J10">
+        <v>431.24099999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify the code to initialize the output buffer with the multithreading fashion.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\research\CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC4E3C8-EBF3-4665-BFC8-2DAD21C81B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FECE546-B085-46F9-A668-389E5E8508AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>noBlock_singleThread</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +68,10 @@
   </si>
   <si>
     <t>loop unrolling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GOP/s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -395,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -407,15 +419,18 @@
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.9140625" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.9140625" customWidth="1"/>
+    <col min="11" max="11" width="14.08203125" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="J1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -431,11 +446,17 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -454,11 +475,19 @@
       <c r="H3">
         <v>49175.35</v>
       </c>
-      <c r="J3">
+      <c r="I3">
+        <f>16*16*128*128*4*4*2/H3*1000/1000000000</f>
+        <v>2.7293700604062812E-3</v>
+      </c>
+      <c r="K3">
         <v>2817.8130000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3">
+        <f>16*16*128*128*4*4*2/K3*1000/1000000000</f>
+        <v>4.7631879049461409E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -477,11 +506,19 @@
       <c r="H4">
         <v>6597.8890000000001</v>
       </c>
-      <c r="J4">
+      <c r="I4">
+        <f t="shared" ref="I4:I10" si="0">16*16*128*128*4*4*2/H4*1000/1000000000</f>
+        <v>2.0342525920032908E-2</v>
+      </c>
+      <c r="K4">
         <v>461.50299999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4">
+        <f t="shared" ref="L4:L10" si="1">16*16*128*128*4*4*2/K4*1000/1000000000</f>
+        <v>0.29082742257363442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -500,11 +537,19 @@
       <c r="H5">
         <v>5134.2669999999998</v>
       </c>
-      <c r="J5">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2.6141555941675804E-2</v>
+      </c>
+      <c r="K5">
         <v>374.96</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>0.35795212289310868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="E6">
         <v>16</v>
       </c>
@@ -517,11 +562,19 @@
       <c r="H6">
         <v>6027.4160000000002</v>
       </c>
-      <c r="J6">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>2.2267872003525226E-2</v>
+      </c>
+      <c r="K6">
         <v>380.839</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>0.35242642691531068</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="E8">
         <v>8</v>
       </c>
@@ -534,11 +587,19 @@
       <c r="H8">
         <v>6140.1120000000001</v>
       </c>
-      <c r="J8">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>2.1859166086872682E-2</v>
+      </c>
+      <c r="K8">
         <v>398.89299999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0.33647551599050374</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="D9" s="1"/>
       <c r="E9">
         <v>4</v>
@@ -552,11 +613,19 @@
       <c r="H9">
         <v>5153.28</v>
       </c>
-      <c r="J9">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>2.6045106805762545E-2</v>
+      </c>
+      <c r="K9">
         <v>377.12</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>0.35590190920661857</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="E10">
         <v>2</v>
       </c>
@@ -569,8 +638,16 @@
       <c r="H10">
         <v>6513.1080000000002</v>
       </c>
-      <c r="J10">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>2.0607324183784456E-2</v>
+      </c>
+      <c r="K10">
         <v>431.24099999999999</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>0.31123600956309816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the local size back to Tm Tr Tc
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\research\CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FECE546-B085-46F9-A668-389E5E8508AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C792241-A076-481A-B39C-564B703C97AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -409,14 +407,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="21.9140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.9140625" customWidth="1"/>
     <col min="9" max="9" width="13.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
Nonblocking version not working for hardware for now.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\research\CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C792241-A076-481A-B39C-564B703C97AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C62794-0891-4B6D-BA78-C5A836BA0CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>noBlock_singleThread</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,10 +63,6 @@
   </si>
   <si>
     <t>Kernel time (ms)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loop unrolling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -93,18 +90,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -124,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -405,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -424,12 +415,10 @@
     <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    <row r="1" spans="1:11">
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -446,21 +435,12 @@
         <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B3">
-        <v>2876184.915</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -472,26 +452,16 @@
         <v>2</v>
       </c>
       <c r="H3">
-        <v>49175.35</v>
+        <v>1768874.44</v>
       </c>
       <c r="I3">
         <f>16*16*128*128*4*4*2/H3*1000/1000000000</f>
-        <v>2.7293700604062812E-3</v>
-      </c>
-      <c r="K3">
-        <v>2817.8130000000001</v>
-      </c>
-      <c r="L3">
-        <f>16*16*128*128*4*4*2/K3*1000/1000000000</f>
-        <v>4.7631879049461409E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
+        <v>7.5877476074559595E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1149000.395</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -503,26 +473,16 @@
         <v>4</v>
       </c>
       <c r="H4">
-        <v>6597.8890000000001</v>
+        <v>221633.89799999999</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I10" si="0">16*16*128*128*4*4*2/H4*1000/1000000000</f>
-        <v>2.0342525920032908E-2</v>
-      </c>
-      <c r="K4">
-        <v>461.50299999999999</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L10" si="1">16*16*128*128*4*4*2/K4*1000/1000000000</f>
-        <v>0.29082742257363442</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
+        <v>6.055830322489749E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1091610.7679999999</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -534,21 +494,14 @@
         <v>8</v>
       </c>
       <c r="H5">
-        <v>5134.2669999999998</v>
+        <v>27881.647000000001</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>2.6141555941675804E-2</v>
-      </c>
-      <c r="K5">
-        <v>374.96</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="1"/>
-        <v>0.35795212289310868</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>4.8138378625911154E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="E6">
         <v>16</v>
       </c>
@@ -559,21 +512,14 @@
         <v>16</v>
       </c>
       <c r="H6">
-        <v>6027.4160000000002</v>
+        <v>3489.7469999999998</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>2.2267872003525226E-2</v>
-      </c>
-      <c r="K6">
-        <v>380.839</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
-        <v>0.35242642691531068</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>3.8460589836455193E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="E8">
         <v>8</v>
       </c>
@@ -584,21 +530,14 @@
         <v>64</v>
       </c>
       <c r="H8">
-        <v>6140.1120000000001</v>
+        <v>3516.3539999999998</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>2.1859166086872682E-2</v>
-      </c>
-      <c r="K8">
-        <v>398.89299999999997</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>0.33647551599050374</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>3.8169572233057315E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="D9" s="1"/>
       <c r="E9">
         <v>4</v>
@@ -610,21 +549,14 @@
         <v>32</v>
       </c>
       <c r="H9">
-        <v>5153.28</v>
+        <v>27818.054</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>2.6045106805762545E-2</v>
-      </c>
-      <c r="K9">
-        <v>377.12</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
-        <v>0.35590190920661857</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>4.8248424566290646E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="E10">
         <v>2</v>
       </c>
@@ -635,18 +567,11 @@
         <v>16</v>
       </c>
       <c r="H10">
-        <v>6513.1080000000002</v>
+        <v>221552.06899999999</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>2.0607324183784456E-2</v>
-      </c>
-      <c r="K10">
-        <v>431.24099999999999</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>0.31123600956309816</v>
+        <v>6.0580670090695484E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sanitized global work size
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\research\CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B7913D-3F88-4C93-B9BF-C4814365C68A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B8EBC-C669-4737-8A7B-63CA152D458E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -508,9 +508,12 @@
       <c r="G6">
         <v>16</v>
       </c>
-      <c r="I6" t="e">
+      <c r="H6">
+        <v>2987.895</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4.4920496871543342E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11">

</xml_diff>

<commit_message>
Added script to test performance of the blocking version
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\research\CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B8EBC-C669-4737-8A7B-63CA152D458E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3836F2A2-8166-46EE-AD9A-EA3C8F95B086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>noBlock_singleThread</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +67,14 @@
   </si>
   <si>
     <t>GOP/s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed buffer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -90,12 +98,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,12 +124,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -398,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -416,12 +431,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11">
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
@@ -435,6 +456,12 @@
         <v>7</v>
       </c>
       <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -442,6 +469,9 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
       <c r="E3">
         <v>2</v>
       </c>
@@ -455,11 +485,17 @@
         <f>16*16*128*128*4*4*2/H3*1000/1000000000</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="J3">
+        <v>7807.82</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
       <c r="E4">
         <v>4</v>
       </c>
@@ -476,11 +512,17 @@
         <f t="shared" ref="I4:I10" si="0">16*16*128*128*4*4*2/H4*1000/1000000000</f>
         <v>0.14930948256969728</v>
       </c>
+      <c r="J4">
+        <v>5519.6459999999997</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
       <c r="E5">
         <v>8</v>
       </c>
@@ -497,8 +539,14 @@
         <f t="shared" si="0"/>
         <v>0.18996990606082481</v>
       </c>
+      <c r="J5">
+        <v>4905.6850000000004</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="D6">
+        <v>6</v>
+      </c>
       <c r="E6">
         <v>16</v>
       </c>
@@ -517,6 +565,9 @@
       </c>
     </row>
     <row r="8" spans="1:11">
+      <c r="D8">
+        <v>6</v>
+      </c>
       <c r="E8">
         <v>8</v>
       </c>
@@ -535,7 +586,9 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="D9" s="1"/>
+      <c r="D9" s="3">
+        <v>6</v>
+      </c>
       <c r="E9">
         <v>4</v>
       </c>
@@ -545,12 +598,21 @@
       <c r="G9">
         <v>32</v>
       </c>
-      <c r="I9" t="e">
+      <c r="H9">
+        <v>2716.6819999999998</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4.9405019799888254E-2</v>
+      </c>
+      <c r="J9">
+        <v>4749.9260000000004</v>
       </c>
     </row>
     <row r="10" spans="1:11">
+      <c r="D10">
+        <v>6</v>
+      </c>
       <c r="E10">
         <v>2</v>
       </c>

</xml_diff>